<commit_message>
Modificaciones en equipo de trabajo y estimación sin terminar
</commit_message>
<xml_diff>
--- a/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
+++ b/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
@@ -11,8 +11,43 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+  <si>
+    <t>WBS Nivel 2</t>
+  </si>
+  <si>
+    <t>WBS Hojas</t>
+  </si>
+  <si>
+    <t>Infraestructura</t>
+  </si>
+  <si>
+    <t>Requerimientos de infraestructura</t>
+  </si>
+  <si>
+    <t>Curso UARTN (Material)</t>
+  </si>
+  <si>
+    <t>Módulo administración de alumnos</t>
+  </si>
+  <si>
+    <t>Módulo administración de docentes</t>
+  </si>
+  <si>
+    <t>Curso UARTN (Dictado)</t>
+  </si>
+  <si>
+    <t>Módulo administración de usuarios, roles y permisos</t>
+  </si>
+  <si>
+    <t>Curso UARTN (Planificación curso)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +87,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -60,7 +119,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Oficina">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Oficina">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -168,7 +227,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Oficina">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -342,12 +401,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="21" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" ht="21" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="21" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="21" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="21" customHeight="1">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A3:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Terminé estimacion uartn capacitación
</commit_message>
<xml_diff>
--- a/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
+++ b/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>WBS Nivel 2</t>
   </si>
@@ -24,12 +24,6 @@
     <t>WBS Hojas</t>
   </si>
   <si>
-    <t>Infraestructura</t>
-  </si>
-  <si>
-    <t>Requerimientos de infraestructura</t>
-  </si>
-  <si>
     <t>Curso UARTN (Material)</t>
   </si>
   <si>
@@ -39,20 +33,77 @@
     <t>Módulo administración de docentes</t>
   </si>
   <si>
-    <t>Curso UARTN (Dictado)</t>
-  </si>
-  <si>
     <t>Módulo administración de usuarios, roles y permisos</t>
   </si>
   <si>
-    <t>Curso UARTN (Planificación curso)</t>
+    <t>Módulo administración de carreras</t>
+  </si>
+  <si>
+    <t>Módulo administración de materias</t>
+  </si>
+  <si>
+    <t>Módulo administración de cursos</t>
+  </si>
+  <si>
+    <t>Módulo administración de correlatividades</t>
+  </si>
+  <si>
+    <t>Administrador de infraestructura</t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t>Planificación</t>
+  </si>
+  <si>
+    <t>Administración proyecto</t>
+  </si>
+  <si>
+    <t>Dictado del curso</t>
+  </si>
+  <si>
+    <t>Porcentaje dictado</t>
+  </si>
+  <si>
+    <t>Porcentaje Planificacion</t>
+  </si>
+  <si>
+    <t>Porcentaje análisis</t>
+  </si>
+  <si>
+    <t>porcentaje administración infraestructura</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total entrega 1</t>
+  </si>
+  <si>
+    <t>Total entrega 2</t>
+  </si>
+  <si>
+    <t>Total entrega 3</t>
+  </si>
+  <si>
+    <t>Total capacitación versión</t>
+  </si>
+  <si>
+    <t>Porentaje administración (de la suma de todo)</t>
+  </si>
+  <si>
+    <t>algo tendría que ir aca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,8 +111,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,8 +132,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -83,28 +159,424 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -401,107 +873,444 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47.42578125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="14">
+        <f>ROUNDUP(H2/100*C19,0)</f>
+        <v>12</v>
+      </c>
+      <c r="D2" s="14">
+        <f>ROUNDUP(H2/100*C18,0)</f>
+        <v>48</v>
+      </c>
+      <c r="E2" s="14">
+        <f>ROUNDUP(C17*(C2+D2+F2+G2+H2)/100,0)</f>
+        <v>44</v>
+      </c>
+      <c r="F2" s="14">
+        <f>ROUNDUP(H2/100*C16,0)</f>
+        <v>12</v>
+      </c>
+      <c r="G2" s="14">
+        <f>ROUNDUP(H2/100*C15, 0)</f>
+        <v>24</v>
+      </c>
+      <c r="H2" s="15">
+        <f>100*1.2</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="14">
+        <f>ROUNDUP(H3/100*C19,0)</f>
+        <v>10</v>
+      </c>
+      <c r="D3" s="14">
+        <f>ROUNDUP(H3/100*C18,0)</f>
+        <v>39</v>
+      </c>
+      <c r="E3" s="14">
+        <f>ROUNDUP(C17*(C3+D3+F3+G3+H3)/100,0)</f>
+        <v>35</v>
+      </c>
+      <c r="F3" s="14">
+        <f>ROUNDUP(H3/100*C16,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G3" s="14">
+        <f>ROUNDUP(H3/100*C15,0)</f>
+        <v>20</v>
+      </c>
+      <c r="H3" s="16">
+        <f>80*1.2</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="14">
+        <f>ROUNDUP(H4/100*C19,0)</f>
+        <v>5</v>
+      </c>
+      <c r="D4" s="14">
+        <f>ROUNDUP(H4/100*C18,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E4" s="14">
+        <f>ROUNDUP(C17*(C4+D4+F4+G4+H4)/100,0)</f>
+        <v>18</v>
+      </c>
+      <c r="F4" s="14">
+        <f>ROUNDUP(H4/100*C16,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G4" s="14">
+        <f>ROUNDUP(H4/100*C15, 0)</f>
+        <v>10</v>
+      </c>
+      <c r="H4" s="18">
+        <f>40*1.2</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="14">
+        <f>ROUNDUP(H5/100*C19,0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="14">
+        <f>ROUNDUP(H5/100*C18,0)</f>
+        <v>29</v>
+      </c>
+      <c r="E5" s="14">
+        <f>ROUNDUP(C17*(C5+D5+F5+G5+H5)/100,0)</f>
+        <v>27</v>
+      </c>
+      <c r="F5" s="14">
+        <f>ROUNDUP(H5/100*C16,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G5" s="14">
+        <f>ROUNDUP(H5/100*C15, 0)</f>
+        <v>15</v>
+      </c>
+      <c r="H5" s="15">
+        <f>60*1.2</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="14">
+        <f>ROUNDUP(H6/100*C19,0)</f>
+        <v>8</v>
+      </c>
+      <c r="D6" s="14">
+        <f>ROUNDUP(H6/100*C18,0)</f>
+        <v>29</v>
+      </c>
+      <c r="E6" s="14">
+        <f>ROUNDUP(C17*(C6+D6+F6+G6+H6)/100,0)</f>
+        <v>27</v>
+      </c>
+      <c r="F6" s="14">
+        <f>ROUNDUP(H6/100*C16,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G6" s="14">
+        <f>ROUNDUP(H6/100*C15,0)</f>
+        <v>15</v>
+      </c>
+      <c r="H6" s="18">
+        <f>60*1.2</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="14">
+        <f>ROUNDUP(H7/100*C19,0)</f>
+        <v>10</v>
+      </c>
+      <c r="D7" s="14">
+        <f>ROUNDUP(H7/100*C18,0)</f>
+        <v>39</v>
+      </c>
+      <c r="E7" s="14">
+        <f>ROUNDUP(C17*(C7+D7+F7+G7+H7)/100,0)</f>
+        <v>35</v>
+      </c>
+      <c r="F7" s="14">
+        <f>ROUNDUP(H7/100*C16,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G7" s="14">
+        <f>ROUNDUP(H7/100*C15,0)</f>
+        <v>20</v>
+      </c>
+      <c r="H7" s="15">
+        <f>80*1.2</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C8" s="14">
+        <f>ROUNDUP(H8/100*C19,0)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="21" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="21" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="D8" s="14">
+        <f>ROUNDUP(H8/100*C18,0)</f>
+        <v>20</v>
+      </c>
+      <c r="E8" s="14">
+        <f>ROUNDUP(C17*(C8+D8+F8+G8+H8)/100,0)</f>
+        <v>18</v>
+      </c>
+      <c r="F8" s="14">
+        <f>ROUNDUP(H8/100*C16,0)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="21" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="21" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
+      <c r="G8" s="14">
+        <f>ROUNDUP(H8/100*C15,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="20">
+        <f>40*1.2</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="B9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="21">
+        <f>SUM(C2:C4)</f>
+        <v>27</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="shared" ref="D9:H9" si="0">SUM(D2:D4)</f>
+        <v>107</v>
+      </c>
+      <c r="E9" s="21">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="B10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="21">
+        <f>SUM(C5:C6)</f>
+        <v>16</v>
+      </c>
+      <c r="D10" s="21">
+        <f t="shared" ref="D10:H10" si="1">SUM(D5:D6)</f>
+        <v>58</v>
+      </c>
+      <c r="E10" s="21">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F10" s="21">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1">
+      <c r="B11" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="21">
+        <f>SUM(C7:C8)</f>
+        <v>15</v>
+      </c>
+      <c r="D11" s="21">
+        <f>SUM(D7:D8)</f>
+        <v>59</v>
+      </c>
+      <c r="E11" s="21">
+        <f>SUM(E7:E8)</f>
+        <v>53</v>
+      </c>
+      <c r="F11" s="21">
+        <f>SUM(F7:F8)</f>
+        <v>15</v>
+      </c>
+      <c r="G11" s="21">
+        <v>0</v>
+      </c>
+      <c r="H11" s="21">
+        <f>SUM(H7:H8)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1">
+      <c r="B12" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="22">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <f>SUM(G2:G9)</f>
+        <v>114</v>
+      </c>
+      <c r="H12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" thickBot="1">
+      <c r="B13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="23">
+        <f>SUM(C2:C8)</f>
+        <v>58</v>
+      </c>
+      <c r="D13" s="17">
+        <f>SUM(D2:D8)</f>
+        <v>224</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" ref="E13:H13" si="2">SUM(E2:E8)</f>
+        <v>204</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="H13" s="17">
+        <f t="shared" si="2"/>
+        <v>552</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" thickBot="1"/>
+    <row r="15" spans="1:8" ht="21" customHeight="1">
+      <c r="B15" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="21" customHeight="1">
+      <c r="B16" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="21" customHeight="1">
+      <c r="B17" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="19.5" customHeight="1">
+      <c r="B18" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="21" customHeight="1" thickBot="1">
+      <c r="B19" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="32">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A3:A5"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
estimación y planificación UARTN Capacitación
</commit_message>
<xml_diff>
--- a/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
+++ b/UARTN Capacitación/Estimación Sistema UARTN Capacitación.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +261,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -300,7 +307,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -754,11 +761,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -913,6 +944,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="11" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1219,17 +1266,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1238,7 +1285,7 @@
     <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" thickBot="1">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1312,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="74" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1296,7 +1343,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
@@ -1325,7 +1372,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="74"/>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1354,7 +1401,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A5" s="68"/>
+      <c r="A5" s="74"/>
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1430,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A6" s="68"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
@@ -1412,7 +1459,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A7" s="68"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="17" t="s">
         <v>8</v>
       </c>
@@ -1441,7 +1488,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" customHeight="1" thickBot="1">
-      <c r="A8" s="69"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1679,18 +1726,27 @@
       <c r="B25" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="71"/>
+      <c r="E25" s="71" t="s">
         <v>54</v>
       </c>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
     </row>
     <row r="26" spans="1:8" ht="21" customHeight="1">
       <c r="B26" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="C26" s="69"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1698,13 +1754,16 @@
       <c r="B27" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="69"/>
+      <c r="D27" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="E27" s="68"/>
+      <c r="F27" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="G27" s="68"/>
+      <c r="H27" s="68" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1712,23 +1771,31 @@
       <c r="B28" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="69"/>
+      <c r="D28" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68" t="s">
         <v>54</v>
       </c>
+      <c r="H28" s="68"/>
     </row>
     <row r="29" spans="1:8" ht="21" customHeight="1" thickBot="1">
       <c r="B29" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="69"/>
+      <c r="D29" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68" t="s">
         <v>54</v>
       </c>
+      <c r="H29" s="68"/>
     </row>
     <row r="30" spans="1:8" ht="21" customHeight="1" thickBot="1"/>
     <row r="31" spans="1:8" ht="21" customHeight="1" thickBot="1">
@@ -1741,15 +1808,18 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="21" customHeight="1">
+    <row r="33" spans="1:2" ht="21" customHeight="1">
       <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="50.25" customHeight="1">
+    <row r="34" spans="1:2" ht="50.25" customHeight="1">
       <c r="B34" s="1" t="s">
         <v>58</v>
       </c>
+    </row>
+    <row r="44" spans="1:2" ht="21" customHeight="1">
+      <c r="A44" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1763,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="A1:N27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1786,30 +1856,30 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="32"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="70" t="s">
+      <c r="E1" s="77"/>
+      <c r="F1" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="71"/>
-      <c r="H1" s="70" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="71"/>
-      <c r="J1" s="70" t="s">
+      <c r="I1" s="77"/>
+      <c r="J1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="71"/>
-      <c r="L1" s="70" t="s">
+      <c r="K1" s="77"/>
+      <c r="L1" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="71"/>
+      <c r="M1" s="77"/>
       <c r="N1" s="61" t="s">
         <v>32</v>
       </c>
@@ -2253,7 +2323,7 @@
       <c r="M16" s="58"/>
       <c r="N16" s="45"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:18">
       <c r="A17" s="33" t="s">
         <v>42</v>
       </c>
@@ -2277,7 +2347,7 @@
       <c r="M17" s="58"/>
       <c r="N17" s="45"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:18">
       <c r="A18" s="33" t="s">
         <v>40</v>
       </c>
@@ -2303,7 +2373,7 @@
       <c r="M18" s="57"/>
       <c r="N18" s="44"/>
     </row>
-    <row r="19" spans="1:14" ht="71.25">
+    <row r="19" spans="1:18" ht="71.25">
       <c r="D19" s="44"/>
       <c r="E19" s="55" t="s">
         <v>35</v>
@@ -2324,12 +2394,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:18">
       <c r="A22" s="65" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="R22" s="72"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -2386,7 +2457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:18">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2514,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:18">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2500,7 +2571,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2557,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:18">
       <c r="A27" t="s">
         <v>43</v>
       </c>

</xml_diff>